<commit_message>
try formatted str for dates
</commit_message>
<xml_diff>
--- a/Start/Ch2/NewWorkbook.xlsx
+++ b/Start/Ch2/NewWorkbook.xlsx
@@ -17,9 +17,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -49,9 +47,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,40 +431,42 @@
       <c r="B1" t="n">
         <v>123.4567</v>
       </c>
-      <c r="C1" s="1" t="n">
-        <v>47574</v>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>2030-04-01</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C5" t="n">
+        <v>37</v>
+      </c>
+      <c r="D5" t="n">
+        <v>44</v>
+      </c>
+      <c r="E5" t="n">
+        <v>20</v>
+      </c>
+      <c r="F5" t="n">
         <v>49</v>
       </c>
-      <c r="D5" t="n">
-        <v>48</v>
-      </c>
-      <c r="E5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F5" t="n">
-        <v>38</v>
-      </c>
       <c r="G5" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H5" t="n">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="I5" t="n">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="J5" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>